<commit_message>
feat: create activity when add revenue
</commit_message>
<xml_diff>
--- a/db/seeds/excel/seeds.xlsx
+++ b/db/seeds/excel/seeds.xlsx
@@ -8,8 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\freelance\digihub\db\seeds\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A468DA2-6E15-48CE-9871-133BBBC83044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" activeTab="5"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="7" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3889" uniqueCount="380">
   <si>
     <t>ID</t>
   </si>
@@ -1175,8 +1176,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1209,6 +1210,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1255,34 +1264,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="3" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 2 10" xfId="2"/>
-    <cellStyle name="Normal 83 3 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2 10" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 83 3 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1295,7 +1305,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1559,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6A588D-8D75-4D77-B1BB-2F8EFE21D9F0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1570,10 +1580,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1611,7 +1621,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1621,10 +1631,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1646,7 +1656,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B5"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1656,10 +1666,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1705,7 +1715,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1715,13 +1725,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1910,8 +1920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE61A12-731F-4E64-A738-8484293B7E52}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1921,10 +1931,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2225,44 +2235,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672936D5-D2E7-4DCD-8047-B176548ED4E4}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col customWidth="true" max="2" min="2" width="21.33203125"/>
-    <col customWidth="true" max="3" min="3" width="16.59765625"/>
-    <col customWidth="true" max="4" min="4" width="15"/>
-    <col customWidth="true" max="5" min="5" width="13.46484375"/>
-    <col customWidth="true" max="6" min="6" width="29.06640625"/>
-    <col customWidth="true" max="7" min="7" width="13.9296875"/>
+    <col min="1" max="1" width="30.73046875" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="13.46484375" customWidth="1"/>
+    <col min="6" max="6" width="29.06640625" customWidth="1"/>
+    <col min="7" max="7" width="13.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>357</v>
       </c>
@@ -2285,7 +2296,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>358</v>
       </c>
@@ -2308,7 +2319,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>359</v>
       </c>
@@ -2331,7 +2342,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>360</v>
       </c>
@@ -2354,7 +2365,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>361</v>
       </c>
@@ -2377,7 +2388,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>362</v>
       </c>
@@ -2400,7 +2411,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>363</v>
       </c>
@@ -2423,7 +2434,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>364</v>
       </c>
@@ -2446,7 +2457,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>365</v>
       </c>
@@ -2469,7 +2480,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>366</v>
       </c>
@@ -2492,7 +2503,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>367</v>
       </c>
@@ -2515,7 +2526,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>368</v>
       </c>
@@ -2538,7 +2549,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>369</v>
       </c>
@@ -2561,7 +2572,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>370</v>
       </c>
@@ -2584,7 +2595,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>371</v>
       </c>
@@ -2607,7 +2618,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>372</v>
       </c>
@@ -2630,7 +2641,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>373</v>
       </c>
@@ -2653,7 +2664,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>374</v>
       </c>
@@ -2676,7 +2687,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>379</v>
       </c>
@@ -2695,7 +2706,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F20" r:id="rId1"/>
+    <hyperlink ref="F20" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2705,15 +2716,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA38801E-1A60-4864-8E10-0B0AB49BCEEA}">
   <dimension ref="A1:G1200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1200" sqref="B1200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="13.06640625" customWidth="1"/>
     <col min="6" max="6" width="13.53125" customWidth="1"/>
-    <col min="7" max="7" width="11.73046875" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
chore: add vehicle types
</commit_message>
<xml_diff>
--- a/db/seeds/excel/seeds.xlsx
+++ b/db/seeds/excel/seeds.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\freelance\digihub\db\seeds\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A468DA2-6E15-48CE-9871-133BBBC83044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="7" r:id="rId1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3889" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="386">
   <si>
     <t>ID</t>
   </si>
@@ -1171,13 +1170,31 @@
   </si>
   <si>
     <t>01J8P8RYG80F4X99PDY5WJAAT0</t>
+  </si>
+  <si>
+    <t>ALPHARD</t>
+  </si>
+  <si>
+    <t>VELLFIRE</t>
+  </si>
+  <si>
+    <t>LEXUS</t>
+  </si>
+  <si>
+    <t>01JASYKN22RV3GG764HKT2BEF4</t>
+  </si>
+  <si>
+    <t>01JASYKN6KF6X5JSX8MGV5E31Q</t>
+  </si>
+  <si>
+    <t>01JASYKN9QVQPNN73VBW2WSS6V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1212,7 +1229,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1264,35 +1281,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyFill="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="3" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment wrapText="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 2 10" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 83 3 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 2 10" xfId="2"/>
+    <cellStyle name="Normal 83 3 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1305,7 +1325,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1918,19 +1938,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE61A12-731F-4E64-A738-8484293B7E52}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="true" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="32.46484375" customWidth="1"/>
-    <col min="2" max="2" width="19.86328125" customWidth="1"/>
+    <col customWidth="true" max="1" min="1" width="32.46484375"/>
+    <col customWidth="true" max="2" min="2" width="19.86328125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1938,7 +1958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>321</v>
       </c>
@@ -1946,7 +1966,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>322</v>
       </c>
@@ -1954,7 +1974,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>323</v>
       </c>
@@ -1962,7 +1982,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>324</v>
       </c>
@@ -1970,7 +1990,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>325</v>
       </c>
@@ -1978,7 +1998,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>326</v>
       </c>
@@ -1986,7 +2006,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>327</v>
       </c>
@@ -1994,7 +2014,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>328</v>
       </c>
@@ -2002,7 +2022,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>329</v>
       </c>
@@ -2010,7 +2030,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>330</v>
       </c>
@@ -2018,7 +2038,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>331</v>
       </c>
@@ -2026,7 +2046,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>332</v>
       </c>
@@ -2034,7 +2054,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>333</v>
       </c>
@@ -2042,7 +2062,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>334</v>
       </c>
@@ -2050,7 +2070,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>335</v>
       </c>
@@ -2058,7 +2078,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>336</v>
       </c>
@@ -2066,7 +2086,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>337</v>
       </c>
@@ -2074,7 +2094,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>338</v>
       </c>
@@ -2082,7 +2102,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>339</v>
       </c>
@@ -2090,7 +2110,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>340</v>
       </c>
@@ -2098,7 +2118,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>341</v>
       </c>
@@ -2106,7 +2126,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>342</v>
       </c>
@@ -2114,7 +2134,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>343</v>
       </c>
@@ -2122,7 +2142,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>344</v>
       </c>
@@ -2130,7 +2150,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>345</v>
       </c>
@@ -2138,7 +2158,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>346</v>
       </c>
@@ -2146,7 +2166,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>347</v>
       </c>
@@ -2154,7 +2174,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>348</v>
       </c>
@@ -2162,7 +2182,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>349</v>
       </c>
@@ -2170,7 +2190,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>350</v>
       </c>
@@ -2178,7 +2198,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>351</v>
       </c>
@@ -2186,7 +2206,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>352</v>
       </c>
@@ -2194,7 +2214,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>353</v>
       </c>
@@ -2202,7 +2222,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>354</v>
       </c>
@@ -2210,7 +2230,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>355</v>
       </c>
@@ -2218,12 +2238,36 @@
         <v>266</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>356</v>
       </c>
       <c r="B37" t="s">
         <v>315</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>383</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>384</v>
+      </c>
+      <c r="B39" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>385</v>
+      </c>
+      <c r="B40" t="s">
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2716,7 +2760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA38801E-1A60-4864-8E10-0B0AB49BCEEA}">
   <dimension ref="A1:G1200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1200" sqref="B1200"/>
     </sheetView>
   </sheetViews>

</xml_diff>